<commit_message>
moved some old data to archive
</commit_message>
<xml_diff>
--- a/JCNEx_Test_Progres_Book.xlsx
+++ b/JCNEx_Test_Progres_Book.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Doucments\lubaka\SoftUni\trunk\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="285" yWindow="330" windowWidth="22695" windowHeight="9270" activeTab="1"/>
   </bookViews>
@@ -10,7 +15,7 @@
     <sheet name="Overview" sheetId="5" r:id="rId1"/>
     <sheet name="TESTING PROCESS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -431,12 +436,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="8" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -488,6 +487,12 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="20% - Accent1" xfId="6" builtinId="30"/>
@@ -500,7 +505,37 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="29">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -534,172 +569,6 @@
           <bgColor theme="5"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -907,59 +776,62 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A16:C19" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A16:C19" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <tableColumns count="3">
-    <tableColumn id="1" name="Test Results Summary (Auto Calculated)" dataDxfId="42"/>
-    <tableColumn id="2" name="Number" dataDxfId="41">
+    <tableColumn id="1" name="Test Results Summary (Auto Calculated)" dataDxfId="26"/>
+    <tableColumn id="2" name="Number" dataDxfId="25">
       <calculatedColumnFormula>SUM('TESTING PROCESS'!D2,#REF!,#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Percent" dataDxfId="40" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="Percent" dataDxfId="24" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A3:C5" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A3:C5" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <tableColumns count="3">
-    <tableColumn id="1" name="Reference Information" dataDxfId="37"/>
-    <tableColumn id="2" name="Location" dataDxfId="36"/>
-    <tableColumn id="3" name="Comments" dataDxfId="35"/>
+    <tableColumn id="1" name="Reference Information" dataDxfId="21"/>
+    <tableColumn id="2" name="Location" dataDxfId="20"/>
+    <tableColumn id="3" name="Comments" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A6:C13" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A6:C13" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A6:C13"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Change Log" dataDxfId="32"/>
-    <tableColumn id="2" name="Person" dataDxfId="31"/>
-    <tableColumn id="3" name="Date" dataDxfId="30"/>
+    <tableColumn id="1" name="Change Log" dataDxfId="16"/>
+    <tableColumn id="2" name="Person" dataDxfId="15"/>
+    <tableColumn id="3" name="Date" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:I76" totalsRowShown="0" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:I76" totalsRowShown="0" dataDxfId="9">
   <autoFilter ref="A8:I76"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Test Case ID" dataDxfId="20"/>
-    <tableColumn id="2" name="Test Case Description" dataDxfId="19"/>
-    <tableColumn id="3" name="Expected Result" dataDxfId="18"/>
-    <tableColumn id="4" name="Test Data" dataDxfId="17"/>
-    <tableColumn id="5" name="Actual Result" dataDxfId="16"/>
-    <tableColumn id="6" name="Status" dataDxfId="15"/>
-    <tableColumn id="7" name="Tester" dataDxfId="14"/>
-    <tableColumn id="8" name="Date/Time" dataDxfId="13"/>
-    <tableColumn id="9" name="Comments" dataDxfId="12"/>
+    <tableColumn id="1" name="Test Case ID" dataDxfId="8"/>
+    <tableColumn id="2" name="Test Case Description" dataDxfId="7"/>
+    <tableColumn id="3" name="Expected Result" dataDxfId="6"/>
+    <tableColumn id="4" name="Test Data" dataDxfId="5"/>
+    <tableColumn id="5" name="Actual Result" dataDxfId="4"/>
+    <tableColumn id="6" name="Status" dataDxfId="3"/>
+    <tableColumn id="7" name="Tester" dataDxfId="2"/>
+    <tableColumn id="8" name="Date/Time" dataDxfId="1"/>
+    <tableColumn id="9" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1008,7 +880,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1043,7 +915,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1293,14 +1165,14 @@
       <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
     </row>
     <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -1310,14 +1182,14 @@
         <v>39</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
     </row>
     <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
@@ -1352,92 +1224,92 @@
       <c r="C7" s="8">
         <v>42228</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
     </row>
     <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="9"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
     </row>
     <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="9"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
     </row>
     <row r="10" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="9"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
     </row>
     <row r="11" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="9"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
     </row>
     <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="9"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
     </row>
     <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="9"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
     </row>
     <row r="16" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
@@ -1514,68 +1386,68 @@
   </sheetPr>
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48" style="24" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" style="24" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="24" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="24" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="24"/>
-    <col min="8" max="8" width="15.5703125" style="24" customWidth="1"/>
-    <col min="9" max="9" width="37.85546875" style="24" customWidth="1"/>
+    <col min="2" max="2" width="48" style="22" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" style="22" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="22" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="22"/>
+    <col min="8" max="8" width="15.5703125" style="22" customWidth="1"/>
+    <col min="9" max="9" width="37.85546875" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="I1" s="31"/>
+      <c r="F1" s="20"/>
+      <c r="I1" s="29"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="27">
+      <c r="D2" s="25">
         <v>6</v>
       </c>
-      <c r="F2" s="23"/>
+      <c r="F2" s="21"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="29" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D3" s="25">
         <v>2</v>
       </c>
-      <c r="F3" s="23"/>
+      <c r="F3" s="21"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="29" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="25">
         <v>0</v>
       </c>
     </row>
@@ -1583,1166 +1455,1166 @@
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="22" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-    </row>
-    <row r="10" spans="1:9" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="B9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+    </row>
+    <row r="10" spans="1:9" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="16" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:9" s="14" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="I11" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="19" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+    <row r="12" spans="1:9" s="17" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="25" t="s">
+      <c r="G12" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="H12" s="30" t="s">
+      <c r="H12" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="I12" s="25" t="s">
+      <c r="I12" s="23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="19" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+    <row r="13" spans="1:9" s="17" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="30" t="s">
+      <c r="H13" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="25" t="s">
+      <c r="I13" s="23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="32" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
+    <row r="14" spans="1:9" s="30" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+    <row r="15" spans="1:9" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="I15" s="15" t="s">
+      <c r="I15" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="16" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+    <row r="16" spans="1:9" s="14" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="H16" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="I16" s="15" t="s">
+      <c r="I16" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="16" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:9" s="14" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="18" t="s">
+      <c r="G17" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="I17" s="15" t="s">
+      <c r="I17" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="16" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+    <row r="18" spans="1:9" s="14" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="18" t="s">
+      <c r="G18" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="H18" s="18" t="s">
+      <c r="H18" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="I18" s="15" t="s">
+      <c r="I18" s="13" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="17">
+      <c r="A19" s="15">
         <v>9</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17" t="s">
+      <c r="B19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="17">
+      <c r="A20" s="15">
         <v>10</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17" t="s">
+      <c r="B20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
     </row>
     <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="17">
+      <c r="A21" s="15">
         <v>11</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17" t="s">
+      <c r="B21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-      <c r="B32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="17"/>
-      <c r="B35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
+      <c r="A35" s="15"/>
+      <c r="B35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
-      <c r="B36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
-      <c r="B37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="17"/>
-      <c r="B39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
-      <c r="B40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="17"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="17"/>
-      <c r="B41" s="17"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="17"/>
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
-      <c r="B42" s="17"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="17"/>
+      <c r="A42" s="15"/>
+      <c r="B42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="17"/>
-      <c r="B43" s="17"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="17"/>
+      <c r="A43" s="15"/>
+      <c r="B43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="17"/>
-      <c r="B44" s="17"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="17"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="17"/>
-      <c r="B45" s="17"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="17"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="17"/>
-      <c r="B46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="17"/>
+      <c r="A46" s="15"/>
+      <c r="B46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="17"/>
-      <c r="B47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="17"/>
+      <c r="A47" s="15"/>
+      <c r="B47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
-      <c r="B48" s="17"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17"/>
+      <c r="A48" s="15"/>
+      <c r="B48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="15"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="17"/>
-      <c r="B49" s="17"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
-      <c r="G49" s="17"/>
-      <c r="H49" s="17"/>
-      <c r="I49" s="17"/>
+      <c r="A49" s="15"/>
+      <c r="B49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="17"/>
-      <c r="B50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="17"/>
-      <c r="I50" s="17"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="15"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="17"/>
-      <c r="B51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="17"/>
-      <c r="I51" s="17"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="17"/>
-      <c r="B52" s="17"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="17"/>
-      <c r="G52" s="17"/>
-      <c r="H52" s="17"/>
-      <c r="I52" s="17"/>
+      <c r="A52" s="15"/>
+      <c r="B52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="15"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="17"/>
-      <c r="B53" s="17"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17"/>
-      <c r="G53" s="17"/>
-      <c r="H53" s="17"/>
-      <c r="I53" s="17"/>
+      <c r="A53" s="15"/>
+      <c r="B53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="17"/>
-      <c r="B54" s="17"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="17"/>
-      <c r="G54" s="17"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="17"/>
+      <c r="A54" s="15"/>
+      <c r="B54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="17"/>
-      <c r="B55" s="17"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="17"/>
-      <c r="I55" s="17"/>
+      <c r="A55" s="15"/>
+      <c r="B55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="17"/>
-      <c r="B56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="17"/>
-      <c r="I56" s="17"/>
+      <c r="A56" s="15"/>
+      <c r="B56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="17"/>
-      <c r="B57" s="17"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
-      <c r="G57" s="17"/>
-      <c r="H57" s="17"/>
-      <c r="I57" s="17"/>
+      <c r="A57" s="15"/>
+      <c r="B57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="17"/>
-      <c r="B58" s="17"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="17"/>
-      <c r="H58" s="17"/>
-      <c r="I58" s="17"/>
+      <c r="A58" s="15"/>
+      <c r="B58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="17"/>
-      <c r="B59" s="17"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
-      <c r="I59" s="17"/>
+      <c r="A59" s="15"/>
+      <c r="B59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="15"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="17"/>
-      <c r="B60" s="17"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
-      <c r="G60" s="17"/>
-      <c r="H60" s="17"/>
-      <c r="I60" s="17"/>
+      <c r="A60" s="15"/>
+      <c r="B60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
+      <c r="I60" s="15"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="17"/>
-      <c r="B61" s="17"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="17"/>
-      <c r="I61" s="17"/>
+      <c r="A61" s="15"/>
+      <c r="B61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="15"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="17"/>
-      <c r="B62" s="17"/>
-      <c r="D62" s="17"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="17"/>
-      <c r="G62" s="17"/>
-      <c r="H62" s="17"/>
-      <c r="I62" s="17"/>
+      <c r="A62" s="15"/>
+      <c r="B62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="17"/>
-      <c r="B63" s="17"/>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
-      <c r="G63" s="17"/>
-      <c r="H63" s="17"/>
-      <c r="I63" s="17"/>
+      <c r="A63" s="15"/>
+      <c r="B63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="17"/>
-      <c r="B64" s="17"/>
-      <c r="D64" s="17"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="17"/>
-      <c r="G64" s="17"/>
-      <c r="H64" s="17"/>
-      <c r="I64" s="17"/>
+      <c r="A64" s="15"/>
+      <c r="B64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="15"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="17"/>
-      <c r="B65" s="17"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="17"/>
-      <c r="G65" s="17"/>
-      <c r="H65" s="17"/>
-      <c r="I65" s="17"/>
+      <c r="A65" s="15"/>
+      <c r="B65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="15"/>
+      <c r="I65" s="15"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="17"/>
-      <c r="B66" s="17"/>
-      <c r="D66" s="17"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="17"/>
-      <c r="G66" s="17"/>
-      <c r="H66" s="17"/>
-      <c r="I66" s="17"/>
+      <c r="A66" s="15"/>
+      <c r="B66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="17"/>
-      <c r="B67" s="17"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="17"/>
-      <c r="H67" s="17"/>
-      <c r="I67" s="17"/>
+      <c r="A67" s="15"/>
+      <c r="B67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="15"/>
+      <c r="I67" s="15"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="17"/>
-      <c r="B68" s="17"/>
-      <c r="D68" s="17"/>
-      <c r="E68" s="17"/>
-      <c r="F68" s="17"/>
-      <c r="G68" s="17"/>
-      <c r="H68" s="17"/>
-      <c r="I68" s="17"/>
+      <c r="A68" s="15"/>
+      <c r="B68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="15"/>
+      <c r="I68" s="15"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="17"/>
-      <c r="B69" s="17"/>
-      <c r="D69" s="17"/>
-      <c r="E69" s="17"/>
-      <c r="F69" s="17"/>
-      <c r="G69" s="17"/>
-      <c r="H69" s="17"/>
-      <c r="I69" s="17"/>
+      <c r="A69" s="15"/>
+      <c r="B69" s="15"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="15"/>
+      <c r="F69" s="15"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="15"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="17"/>
-      <c r="B70" s="17"/>
-      <c r="D70" s="17"/>
-      <c r="E70" s="17"/>
-      <c r="F70" s="17"/>
-      <c r="G70" s="17"/>
-      <c r="H70" s="17"/>
-      <c r="I70" s="17"/>
+      <c r="A70" s="15"/>
+      <c r="B70" s="15"/>
+      <c r="D70" s="15"/>
+      <c r="E70" s="15"/>
+      <c r="F70" s="15"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="15"/>
+      <c r="I70" s="15"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="17"/>
-      <c r="B71" s="17"/>
-      <c r="D71" s="17"/>
-      <c r="E71" s="17"/>
-      <c r="F71" s="17"/>
-      <c r="G71" s="17"/>
-      <c r="H71" s="17"/>
-      <c r="I71" s="17"/>
+      <c r="A71" s="15"/>
+      <c r="B71" s="15"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="15"/>
+      <c r="F71" s="15"/>
+      <c r="G71" s="15"/>
+      <c r="H71" s="15"/>
+      <c r="I71" s="15"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="17"/>
-      <c r="B72" s="17"/>
-      <c r="D72" s="17"/>
-      <c r="E72" s="17"/>
-      <c r="F72" s="17"/>
-      <c r="G72" s="17"/>
-      <c r="H72" s="17"/>
-      <c r="I72" s="17"/>
+      <c r="A72" s="15"/>
+      <c r="B72" s="15"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="15"/>
+      <c r="F72" s="15"/>
+      <c r="G72" s="15"/>
+      <c r="H72" s="15"/>
+      <c r="I72" s="15"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="17"/>
-      <c r="B73" s="17"/>
-      <c r="D73" s="17"/>
-      <c r="E73" s="17"/>
-      <c r="F73" s="17"/>
-      <c r="G73" s="17"/>
-      <c r="H73" s="17"/>
-      <c r="I73" s="17"/>
+      <c r="A73" s="15"/>
+      <c r="B73" s="15"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="15"/>
+      <c r="F73" s="15"/>
+      <c r="G73" s="15"/>
+      <c r="H73" s="15"/>
+      <c r="I73" s="15"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="17"/>
-      <c r="B74" s="17"/>
-      <c r="D74" s="17"/>
-      <c r="E74" s="17"/>
-      <c r="F74" s="17"/>
-      <c r="G74" s="17"/>
-      <c r="H74" s="17"/>
-      <c r="I74" s="17"/>
+      <c r="A74" s="15"/>
+      <c r="B74" s="15"/>
+      <c r="D74" s="15"/>
+      <c r="E74" s="15"/>
+      <c r="F74" s="15"/>
+      <c r="G74" s="15"/>
+      <c r="H74" s="15"/>
+      <c r="I74" s="15"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="17"/>
-      <c r="B75" s="17"/>
-      <c r="D75" s="17"/>
-      <c r="E75" s="17"/>
-      <c r="F75" s="17"/>
-      <c r="G75" s="17"/>
-      <c r="H75" s="17"/>
-      <c r="I75" s="17"/>
+      <c r="A75" s="15"/>
+      <c r="B75" s="15"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="15"/>
+      <c r="F75" s="15"/>
+      <c r="G75" s="15"/>
+      <c r="H75" s="15"/>
+      <c r="I75" s="15"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="17"/>
-      <c r="B76" s="17"/>
-      <c r="D76" s="17"/>
-      <c r="E76" s="17"/>
-      <c r="F76" s="17"/>
-      <c r="G76" s="17"/>
-      <c r="H76" s="17"/>
-      <c r="I76" s="17"/>
+      <c r="A76" s="15"/>
+      <c r="B76" s="15"/>
+      <c r="D76" s="15"/>
+      <c r="E76" s="15"/>
+      <c r="F76" s="15"/>
+      <c r="G76" s="15"/>
+      <c r="H76" s="15"/>
+      <c r="I76" s="15"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
-      <c r="B77" s="17"/>
-      <c r="D77" s="17"/>
-      <c r="E77" s="17"/>
-      <c r="F77" s="17"/>
-      <c r="G77" s="17"/>
-      <c r="H77" s="17"/>
-      <c r="I77" s="17"/>
+      <c r="B77" s="15"/>
+      <c r="D77" s="15"/>
+      <c r="E77" s="15"/>
+      <c r="F77" s="15"/>
+      <c r="G77" s="15"/>
+      <c r="H77" s="15"/>
+      <c r="I77" s="15"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
-      <c r="B78" s="17"/>
-      <c r="D78" s="17"/>
-      <c r="E78" s="17"/>
-      <c r="F78" s="17"/>
-      <c r="G78" s="17"/>
-      <c r="H78" s="17"/>
-      <c r="I78" s="17"/>
+      <c r="B78" s="15"/>
+      <c r="D78" s="15"/>
+      <c r="E78" s="15"/>
+      <c r="F78" s="15"/>
+      <c r="G78" s="15"/>
+      <c r="H78" s="15"/>
+      <c r="I78" s="15"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
-      <c r="B79" s="17"/>
-      <c r="D79" s="17"/>
-      <c r="E79" s="17"/>
-      <c r="F79" s="17"/>
-      <c r="G79" s="17"/>
-      <c r="H79" s="17"/>
-      <c r="I79" s="17"/>
+      <c r="B79" s="15"/>
+      <c r="D79" s="15"/>
+      <c r="E79" s="15"/>
+      <c r="F79" s="15"/>
+      <c r="G79" s="15"/>
+      <c r="H79" s="15"/>
+      <c r="I79" s="15"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
-      <c r="B80" s="17"/>
-      <c r="D80" s="17"/>
-      <c r="E80" s="17"/>
-      <c r="F80" s="17"/>
-      <c r="G80" s="17"/>
-      <c r="H80" s="17"/>
-      <c r="I80" s="17"/>
+      <c r="B80" s="15"/>
+      <c r="D80" s="15"/>
+      <c r="E80" s="15"/>
+      <c r="F80" s="15"/>
+      <c r="G80" s="15"/>
+      <c r="H80" s="15"/>
+      <c r="I80" s="15"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
-      <c r="B81" s="17"/>
-      <c r="D81" s="17"/>
-      <c r="E81" s="17"/>
-      <c r="F81" s="17"/>
-      <c r="G81" s="17"/>
-      <c r="H81" s="17"/>
-      <c r="I81" s="17"/>
+      <c r="B81" s="15"/>
+      <c r="D81" s="15"/>
+      <c r="E81" s="15"/>
+      <c r="F81" s="15"/>
+      <c r="G81" s="15"/>
+      <c r="H81" s="15"/>
+      <c r="I81" s="15"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
-      <c r="B82" s="17"/>
-      <c r="D82" s="17"/>
-      <c r="E82" s="17"/>
-      <c r="F82" s="17"/>
-      <c r="G82" s="17"/>
-      <c r="H82" s="17"/>
-      <c r="I82" s="17"/>
+      <c r="B82" s="15"/>
+      <c r="D82" s="15"/>
+      <c r="E82" s="15"/>
+      <c r="F82" s="15"/>
+      <c r="G82" s="15"/>
+      <c r="H82" s="15"/>
+      <c r="I82" s="15"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
-      <c r="B83" s="17"/>
-      <c r="D83" s="17"/>
-      <c r="E83" s="17"/>
-      <c r="F83" s="17"/>
-      <c r="G83" s="17"/>
-      <c r="H83" s="17"/>
-      <c r="I83" s="17"/>
+      <c r="B83" s="15"/>
+      <c r="D83" s="15"/>
+      <c r="E83" s="15"/>
+      <c r="F83" s="15"/>
+      <c r="G83" s="15"/>
+      <c r="H83" s="15"/>
+      <c r="I83" s="15"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
-      <c r="B84" s="17"/>
-      <c r="D84" s="17"/>
-      <c r="E84" s="17"/>
-      <c r="F84" s="17"/>
-      <c r="G84" s="17"/>
-      <c r="H84" s="17"/>
-      <c r="I84" s="17"/>
+      <c r="B84" s="15"/>
+      <c r="D84" s="15"/>
+      <c r="E84" s="15"/>
+      <c r="F84" s="15"/>
+      <c r="G84" s="15"/>
+      <c r="H84" s="15"/>
+      <c r="I84" s="15"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
-      <c r="B85" s="17"/>
-      <c r="D85" s="17"/>
-      <c r="E85" s="17"/>
-      <c r="F85" s="17"/>
-      <c r="G85" s="17"/>
-      <c r="H85" s="17"/>
-      <c r="I85" s="17"/>
+      <c r="B85" s="15"/>
+      <c r="D85" s="15"/>
+      <c r="E85" s="15"/>
+      <c r="F85" s="15"/>
+      <c r="G85" s="15"/>
+      <c r="H85" s="15"/>
+      <c r="I85" s="15"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
-      <c r="B86" s="17"/>
-      <c r="D86" s="17"/>
-      <c r="E86" s="17"/>
-      <c r="F86" s="17"/>
-      <c r="G86" s="17"/>
-      <c r="H86" s="17"/>
-      <c r="I86" s="17"/>
+      <c r="B86" s="15"/>
+      <c r="D86" s="15"/>
+      <c r="E86" s="15"/>
+      <c r="F86" s="15"/>
+      <c r="G86" s="15"/>
+      <c r="H86" s="15"/>
+      <c r="I86" s="15"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
-      <c r="B87" s="17"/>
-      <c r="D87" s="17"/>
-      <c r="E87" s="17"/>
-      <c r="F87" s="17"/>
-      <c r="G87" s="17"/>
-      <c r="H87" s="17"/>
-      <c r="I87" s="17"/>
+      <c r="B87" s="15"/>
+      <c r="D87" s="15"/>
+      <c r="E87" s="15"/>
+      <c r="F87" s="15"/>
+      <c r="G87" s="15"/>
+      <c r="H87" s="15"/>
+      <c r="I87" s="15"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
-      <c r="B88" s="17"/>
-      <c r="D88" s="17"/>
-      <c r="E88" s="17"/>
-      <c r="F88" s="17"/>
-      <c r="G88" s="17"/>
-      <c r="H88" s="17"/>
-      <c r="I88" s="17"/>
+      <c r="B88" s="15"/>
+      <c r="D88" s="15"/>
+      <c r="E88" s="15"/>
+      <c r="F88" s="15"/>
+      <c r="G88" s="15"/>
+      <c r="H88" s="15"/>
+      <c r="I88" s="15"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
-      <c r="B89" s="17"/>
-      <c r="D89" s="17"/>
-      <c r="E89" s="17"/>
-      <c r="F89" s="17"/>
-      <c r="G89" s="17"/>
-      <c r="H89" s="17"/>
-      <c r="I89" s="17"/>
+      <c r="B89" s="15"/>
+      <c r="D89" s="15"/>
+      <c r="E89" s="15"/>
+      <c r="F89" s="15"/>
+      <c r="G89" s="15"/>
+      <c r="H89" s="15"/>
+      <c r="I89" s="15"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
-      <c r="B90" s="17"/>
-      <c r="D90" s="17"/>
-      <c r="E90" s="17"/>
-      <c r="F90" s="17"/>
-      <c r="G90" s="17"/>
-      <c r="H90" s="17"/>
-      <c r="I90" s="17"/>
+      <c r="B90" s="15"/>
+      <c r="D90" s="15"/>
+      <c r="E90" s="15"/>
+      <c r="F90" s="15"/>
+      <c r="G90" s="15"/>
+      <c r="H90" s="15"/>
+      <c r="I90" s="15"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
-      <c r="B91" s="17"/>
-      <c r="D91" s="17"/>
-      <c r="E91" s="17"/>
-      <c r="F91" s="17"/>
-      <c r="G91" s="17"/>
-      <c r="H91" s="17"/>
-      <c r="I91" s="17"/>
+      <c r="B91" s="15"/>
+      <c r="D91" s="15"/>
+      <c r="E91" s="15"/>
+      <c r="F91" s="15"/>
+      <c r="G91" s="15"/>
+      <c r="H91" s="15"/>
+      <c r="I91" s="15"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
-      <c r="B92" s="17"/>
-      <c r="D92" s="17"/>
-      <c r="E92" s="17"/>
-      <c r="F92" s="17"/>
-      <c r="G92" s="17"/>
-      <c r="H92" s="17"/>
-      <c r="I92" s="17"/>
+      <c r="B92" s="15"/>
+      <c r="D92" s="15"/>
+      <c r="E92" s="15"/>
+      <c r="F92" s="15"/>
+      <c r="G92" s="15"/>
+      <c r="H92" s="15"/>
+      <c r="I92" s="15"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
-      <c r="B93" s="17"/>
-      <c r="D93" s="17"/>
-      <c r="E93" s="17"/>
-      <c r="F93" s="17"/>
-      <c r="G93" s="17"/>
-      <c r="H93" s="17"/>
-      <c r="I93" s="17"/>
+      <c r="B93" s="15"/>
+      <c r="D93" s="15"/>
+      <c r="E93" s="15"/>
+      <c r="F93" s="15"/>
+      <c r="G93" s="15"/>
+      <c r="H93" s="15"/>
+      <c r="I93" s="15"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
-      <c r="B94" s="17"/>
-      <c r="D94" s="17"/>
-      <c r="E94" s="17"/>
-      <c r="F94" s="17"/>
-      <c r="G94" s="17"/>
-      <c r="H94" s="17"/>
-      <c r="I94" s="17"/>
+      <c r="B94" s="15"/>
+      <c r="D94" s="15"/>
+      <c r="E94" s="15"/>
+      <c r="F94" s="15"/>
+      <c r="G94" s="15"/>
+      <c r="H94" s="15"/>
+      <c r="I94" s="15"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
-      <c r="B95" s="17"/>
-      <c r="D95" s="17"/>
-      <c r="E95" s="17"/>
-      <c r="F95" s="17"/>
-      <c r="G95" s="17"/>
-      <c r="H95" s="17"/>
-      <c r="I95" s="17"/>
+      <c r="B95" s="15"/>
+      <c r="D95" s="15"/>
+      <c r="E95" s="15"/>
+      <c r="F95" s="15"/>
+      <c r="G95" s="15"/>
+      <c r="H95" s="15"/>
+      <c r="I95" s="15"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
-      <c r="B96" s="17"/>
-      <c r="D96" s="17"/>
-      <c r="E96" s="17"/>
-      <c r="F96" s="17"/>
-      <c r="G96" s="17"/>
-      <c r="H96" s="17"/>
-      <c r="I96" s="17"/>
+      <c r="B96" s="15"/>
+      <c r="D96" s="15"/>
+      <c r="E96" s="15"/>
+      <c r="F96" s="15"/>
+      <c r="G96" s="15"/>
+      <c r="H96" s="15"/>
+      <c r="I96" s="15"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
-      <c r="B97" s="17"/>
-      <c r="D97" s="17"/>
-      <c r="E97" s="17"/>
-      <c r="F97" s="17"/>
-      <c r="G97" s="17"/>
-      <c r="H97" s="17"/>
-      <c r="I97" s="17"/>
+      <c r="B97" s="15"/>
+      <c r="D97" s="15"/>
+      <c r="E97" s="15"/>
+      <c r="F97" s="15"/>
+      <c r="G97" s="15"/>
+      <c r="H97" s="15"/>
+      <c r="I97" s="15"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
-      <c r="B98" s="17"/>
-      <c r="D98" s="17"/>
-      <c r="E98" s="17"/>
-      <c r="F98" s="17"/>
-      <c r="G98" s="17"/>
-      <c r="H98" s="17"/>
-      <c r="I98" s="17"/>
+      <c r="B98" s="15"/>
+      <c r="D98" s="15"/>
+      <c r="E98" s="15"/>
+      <c r="F98" s="15"/>
+      <c r="G98" s="15"/>
+      <c r="H98" s="15"/>
+      <c r="I98" s="15"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
-      <c r="B99" s="17"/>
-      <c r="D99" s="17"/>
-      <c r="E99" s="17"/>
-      <c r="F99" s="17"/>
-      <c r="G99" s="17"/>
-      <c r="H99" s="17"/>
-      <c r="I99" s="17"/>
+      <c r="B99" s="15"/>
+      <c r="D99" s="15"/>
+      <c r="E99" s="15"/>
+      <c r="F99" s="15"/>
+      <c r="G99" s="15"/>
+      <c r="H99" s="15"/>
+      <c r="I99" s="15"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
-      <c r="B100" s="17"/>
-      <c r="D100" s="17"/>
-      <c r="E100" s="17"/>
-      <c r="F100" s="17"/>
-      <c r="G100" s="17"/>
-      <c r="H100" s="17"/>
-      <c r="I100" s="17"/>
+      <c r="B100" s="15"/>
+      <c r="D100" s="15"/>
+      <c r="E100" s="15"/>
+      <c r="F100" s="15"/>
+      <c r="G100" s="15"/>
+      <c r="H100" s="15"/>
+      <c r="I100" s="15"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
-      <c r="B101" s="17"/>
-      <c r="D101" s="17"/>
-      <c r="E101" s="17"/>
-      <c r="F101" s="17"/>
-      <c r="G101" s="17"/>
-      <c r="H101" s="17"/>
-      <c r="I101" s="17"/>
+      <c r="B101" s="15"/>
+      <c r="D101" s="15"/>
+      <c r="E101" s="15"/>
+      <c r="F101" s="15"/>
+      <c r="G101" s="15"/>
+      <c r="H101" s="15"/>
+      <c r="I101" s="15"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
-      <c r="B102" s="17"/>
-      <c r="D102" s="17"/>
-      <c r="E102" s="17"/>
-      <c r="F102" s="17"/>
-      <c r="G102" s="17"/>
-      <c r="H102" s="17"/>
-      <c r="I102" s="17"/>
+      <c r="B102" s="15"/>
+      <c r="D102" s="15"/>
+      <c r="E102" s="15"/>
+      <c r="F102" s="15"/>
+      <c r="G102" s="15"/>
+      <c r="H102" s="15"/>
+      <c r="I102" s="15"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
-      <c r="B103" s="17"/>
-      <c r="D103" s="17"/>
-      <c r="E103" s="17"/>
-      <c r="F103" s="17"/>
-      <c r="G103" s="17"/>
-      <c r="H103" s="17"/>
-      <c r="I103" s="17"/>
+      <c r="B103" s="15"/>
+      <c r="D103" s="15"/>
+      <c r="E103" s="15"/>
+      <c r="F103" s="15"/>
+      <c r="G103" s="15"/>
+      <c r="H103" s="15"/>
+      <c r="I103" s="15"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
-      <c r="B104" s="17"/>
-      <c r="D104" s="17"/>
-      <c r="E104" s="17"/>
-      <c r="F104" s="17"/>
-      <c r="G104" s="17"/>
-      <c r="H104" s="17"/>
-      <c r="I104" s="17"/>
+      <c r="B104" s="15"/>
+      <c r="D104" s="15"/>
+      <c r="E104" s="15"/>
+      <c r="F104" s="15"/>
+      <c r="G104" s="15"/>
+      <c r="H104" s="15"/>
+      <c r="I104" s="15"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A19:I76 I10:I11 F10:F11 F12:I12 F13:F14 H13:I14">
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="13" priority="3">
       <formula>$F10="Fail"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="12" priority="4">
       <formula>$F10="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15:F18 I15:I18">
-    <cfRule type="expression" dxfId="9" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>$F15="Fail"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>$F15="Pass"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>